<commit_message>
Character restructure + item, weapon and sword class + camera movement
Changed character spawning
Created Item base class
Created Weapon base class
Created Sword class with basic attack
Created Camera movement
</commit_message>
<xml_diff>
--- a/Documents/TimeSheet.xlsx
+++ b/Documents/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Day</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Trying to understand structure + get basic character with movement</t>
+  </si>
+  <si>
+    <t>29/11</t>
+  </si>
+  <si>
+    <t>Restructuring character + basic sword implementation + camera movement</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -463,6 +469,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enemy spawning + enemy behaviour + basic inventory
-Enemies are now spawned through the character manager
-Enemies can now follow the player and attack when in range + can die
-Set up basic structure for inventory
</commit_message>
<xml_diff>
--- a/Documents/TimeSheet.xlsx
+++ b/Documents/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="912" windowWidth="23040" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="1368" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Day</t>
   </si>
   <si>
-    <t>28/11</t>
-  </si>
-  <si>
     <t>Time spent</t>
   </si>
   <si>
@@ -47,10 +44,13 @@
     <t>Trying to understand structure + get basic character with movement</t>
   </si>
   <si>
-    <t>29/11</t>
-  </si>
-  <si>
     <t>Restructuring character + basic sword implementation + camera movement</t>
+  </si>
+  <si>
+    <t>Spawn enemies through manager + killable enemies</t>
+  </si>
+  <si>
+    <t>Basic inventory + enemy behaviour</t>
   </si>
 </sst>
 </file>
@@ -94,10 +94,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,53 +431,75 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="3">
+        <v>43067</v>
       </c>
       <c r="B2" s="1">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" s="3">
+        <v>43067</v>
       </c>
       <c r="B3" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
+      <c r="A4" s="3">
+        <v>43067</v>
       </c>
       <c r="B4" s="1">
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
+      <c r="A5" s="3">
+        <v>43068</v>
       </c>
       <c r="B5" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43070</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43070</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Consumables + Health potion + Item stat boost on character panel + Inventory update + Spear + Combat text
- Created consumable base class
- Created Health potion
- Character panel now shows equiped stat boost
- Inventory now updates correctly when (un)equiping items
- Created Spear class
- Created basic combat text
</commit_message>
<xml_diff>
--- a/Documents/TimeSheet.xlsx
+++ b/Documents/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2280" windowWidth="23040" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="3192" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Day</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Inventory panel + player sprinting</t>
+  </si>
+  <si>
+    <t>Inventory update when (un)equiping + Spear + Basic combat text</t>
+  </si>
+  <si>
+    <t>Consumable item + Health potion + Character panel show equiped stat boost</t>
   </si>
 </sst>
 </file>
@@ -425,17 +431,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="57.109375" customWidth="1"/>
+    <col min="3" max="3" width="77.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -559,6 +565,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43071</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>43071</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Game complete / over screen + Level design + Shopkeeper stock + God keys
- Implemented screen when game over or completed
- Adjusted level design
- Shopkeeper now has extended base stock
- Implemented god keys to heal / give items
- Nav agent spawn bug fix
- Updated readme
- Time sheed update
</commit_message>
<xml_diff>
--- a/Documents/TimeSheet.xlsx
+++ b/Documents/TimeSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3192" windowWidth="23040" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="3648" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Day</t>
   </si>
@@ -69,6 +69,24 @@
   </si>
   <si>
     <t>Consumable item + Health potion + Character panel show equiped stat boost</t>
+  </si>
+  <si>
+    <t>Basic level design + destructables + Axe + Pick up (Key) + Cuttable Tree + Door locked (item requirement)</t>
+  </si>
+  <si>
+    <t>Created shop + shop panel</t>
+  </si>
+  <si>
+    <t>Show text above shopkeeper and locked door + Locked door remove key on unlock + breakable pot + enemy kill reward</t>
+  </si>
+  <si>
+    <t>Game over / complete screen</t>
+  </si>
+  <si>
+    <t>Update level design</t>
+  </si>
+  <si>
+    <t>Nav agent spawn bug fix + shopkeeper stock and bugfixes + Dev / God keys to heal and give items</t>
   </si>
 </sst>
 </file>
@@ -431,17 +449,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="77.109375" customWidth="1"/>
+    <col min="3" max="3" width="103.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,6 +605,75 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>